<commit_message>
improve seq5in7 algorithm, fast more than 1 time
</commit_message>
<xml_diff>
--- a/data/poker.xlsx
+++ b/data/poker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\r\r_project\20171227_poker\20180211_pk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\r\r_project\20171227_poker\20180211_pk\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,8 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="20170208-10w-3.3hours" sheetId="6" r:id="rId2"/>
-    <sheet name="成牌逻辑" sheetId="10" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="8" r:id="rId4"/>
+    <sheet name="20180219-p2-5w-38min" sheetId="11" r:id="rId3"/>
+    <sheet name="成牌逻辑" sheetId="10" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="159">
   <si>
     <r>
       <t>A</t>
@@ -1039,6 +1040,14 @@
     <t>colSums</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>20170208-10w-3.3hours</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20180219-p2-10w-77.7min</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1047,7 +1056,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1186,6 +1195,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1255,7 +1271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1318,13 +1334,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFB5D2E2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1383,12 +1408,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1422,17 +1441,8 @@
     <xf numFmtId="176" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1488,11 +1498,74 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3312,734 +3385,2082 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:N14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="14" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="6.25" customWidth="1"/>
+    <col min="15" max="15" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="17" max="17" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="30" width="6.375" customWidth="1"/>
+    <col min="31" max="31" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23"/>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21"/>
+      <c r="B1" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="21">
+      <c r="G1" s="57">
         <v>9</v>
       </c>
-      <c r="H1" s="21">
+      <c r="H1" s="57">
         <v>8</v>
       </c>
-      <c r="I1" s="21">
+      <c r="I1" s="57">
         <v>7</v>
       </c>
-      <c r="J1" s="21">
+      <c r="J1" s="57">
         <v>6</v>
       </c>
-      <c r="K1" s="21">
+      <c r="K1" s="57">
         <v>5</v>
       </c>
-      <c r="L1" s="21">
+      <c r="L1" s="57">
         <v>4</v>
       </c>
-      <c r="M1" s="21">
+      <c r="M1" s="57">
         <v>3</v>
       </c>
-      <c r="N1" s="21">
+      <c r="N1" s="57">
         <v>2</v>
       </c>
       <c r="O1" s="19"/>
-    </row>
-    <row r="2" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="Q1" s="55"/>
+      <c r="R1" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="28">
+      <c r="S1" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="T1" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="U1" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="V1" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="W1" s="57">
+        <v>9</v>
+      </c>
+      <c r="X1" s="57">
+        <v>8</v>
+      </c>
+      <c r="Y1" s="57">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="57">
+        <v>6</v>
+      </c>
+      <c r="AA1" s="57">
+        <v>5</v>
+      </c>
+      <c r="AB1" s="57">
+        <v>4</v>
+      </c>
+      <c r="AC1" s="57">
+        <v>3</v>
+      </c>
+      <c r="AD1" s="57">
+        <v>2</v>
+      </c>
+      <c r="AE1" s="58"/>
+    </row>
+    <row r="2" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="26">
         <v>0.85</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="24">
         <v>0.6724</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="24">
         <v>0.66100000000000003</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="24">
         <v>0.6552</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="24">
         <v>0.65780000000000005</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="24">
         <v>0.63249999999999995</v>
       </c>
-      <c r="H2" s="26">
+      <c r="H2" s="24">
         <v>0.62719999999999998</v>
       </c>
-      <c r="I2" s="31">
+      <c r="I2" s="29">
         <v>0.59909999999999997</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="29">
         <v>0.59140000000000004</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="29">
         <v>0.59660000000000002</v>
       </c>
-      <c r="L2" s="31">
+      <c r="L2" s="29">
         <v>0.59330000000000005</v>
       </c>
-      <c r="M2" s="31">
+      <c r="M2" s="29">
         <v>0.59279999999999999</v>
       </c>
-      <c r="N2" s="31">
+      <c r="N2" s="29">
         <v>0.56710000000000005</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="60" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="Q2" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="R2" s="68">
+        <v>86.2</v>
+      </c>
+      <c r="S2" s="69">
+        <v>68</v>
+      </c>
+      <c r="T2" s="69">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="U2" s="69">
+        <v>67.3</v>
+      </c>
+      <c r="V2" s="69">
+        <v>67</v>
+      </c>
+      <c r="W2" s="69">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="X2" s="69">
+        <v>64.8</v>
+      </c>
+      <c r="Y2" s="69">
+        <v>64.2</v>
+      </c>
+      <c r="Z2" s="69">
+        <v>63.8</v>
+      </c>
+      <c r="AA2" s="69">
+        <v>63.4</v>
+      </c>
+      <c r="AB2" s="69">
+        <v>63.1</v>
+      </c>
+      <c r="AC2" s="69">
+        <v>63</v>
+      </c>
+      <c r="AD2" s="69">
+        <v>63.1</v>
+      </c>
+      <c r="AE2" s="60" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="24">
         <v>0.64490000000000003</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="26">
         <v>0.82</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="24">
         <v>0.63129999999999997</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>0.62919999999999998</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="24">
         <v>0.62929999999999997</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="24">
         <v>0.60470000000000002</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="29">
         <v>0.57730000000000004</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="29">
         <v>0.57479999999999998</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="29">
         <v>0.56850000000000001</v>
       </c>
-      <c r="K3" s="31">
+      <c r="K3" s="29">
         <v>0.55740000000000001</v>
       </c>
-      <c r="L3" s="27">
+      <c r="L3" s="25">
         <v>0.53190000000000004</v>
       </c>
-      <c r="M3" s="27">
+      <c r="M3" s="25">
         <v>0.53779999999999994</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="25">
         <v>0.53380000000000005</v>
       </c>
-      <c r="O3" s="33" t="s">
+      <c r="O3" s="60" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="Q3" s="66" t="s">
+        <v>147</v>
+      </c>
+      <c r="R3" s="69">
+        <v>66.7</v>
+      </c>
+      <c r="S3" s="68">
+        <v>80.8</v>
+      </c>
+      <c r="T3" s="69">
+        <v>63.5</v>
+      </c>
+      <c r="U3" s="69">
+        <v>63.1</v>
+      </c>
+      <c r="V3" s="69">
+        <v>62.7</v>
+      </c>
+      <c r="W3" s="69">
+        <v>61.3</v>
+      </c>
+      <c r="X3" s="71">
+        <v>59.9</v>
+      </c>
+      <c r="Y3" s="71">
+        <v>59.8</v>
+      </c>
+      <c r="Z3" s="71">
+        <v>59.3</v>
+      </c>
+      <c r="AA3" s="71">
+        <v>58.6</v>
+      </c>
+      <c r="AB3" s="71">
+        <v>58.1</v>
+      </c>
+      <c r="AC3" s="71">
+        <v>58</v>
+      </c>
+      <c r="AD3" s="71">
+        <v>58</v>
+      </c>
+      <c r="AE3" s="60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="24">
         <v>0.65490000000000004</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="24">
         <v>0.61150000000000004</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="26">
         <v>0.8</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="24">
         <v>0.6089</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="29">
         <v>0.59799999999999998</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="29">
         <v>0.56740000000000002</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="29">
         <v>0.55810000000000004</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="25">
         <v>0.54310000000000003</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="25">
         <v>0.52839999999999998</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="25">
         <v>0.53539999999999999</v>
       </c>
-      <c r="L4" s="27">
+      <c r="L4" s="25">
         <v>0.52349999999999997</v>
       </c>
-      <c r="M4" s="27">
+      <c r="M4" s="25">
         <v>0.51519999999999999</v>
       </c>
-      <c r="N4" s="27">
+      <c r="N4" s="25">
         <v>0.50039999999999996</v>
       </c>
-      <c r="O4" s="33" t="s">
+      <c r="O4" s="60" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="Q4" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="R4" s="69">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="S4" s="69">
+        <v>61.7</v>
+      </c>
+      <c r="T4" s="68">
+        <v>76.3</v>
+      </c>
+      <c r="U4" s="71">
+        <v>59.5</v>
+      </c>
+      <c r="V4" s="71">
+        <v>59</v>
+      </c>
+      <c r="W4" s="71">
+        <v>57.4</v>
+      </c>
+      <c r="X4" s="71">
+        <v>56.3</v>
+      </c>
+      <c r="Y4" s="71">
+        <v>55.1</v>
+      </c>
+      <c r="Z4" s="72">
+        <v>54.9</v>
+      </c>
+      <c r="AA4" s="72">
+        <v>54.1</v>
+      </c>
+      <c r="AB4" s="72">
+        <v>53.7</v>
+      </c>
+      <c r="AC4" s="72">
+        <v>53.5</v>
+      </c>
+      <c r="AD4" s="72">
+        <v>53.5</v>
+      </c>
+      <c r="AE4" s="60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="24">
         <v>0.62980000000000003</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>0.5927</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="29">
         <v>0.58150000000000002</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="26">
         <v>0.77</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="29">
         <v>0.5696</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="29">
         <v>0.55410000000000004</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="25">
         <v>0.53810000000000002</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="25">
         <v>0.51749999999999996</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="25">
         <v>0.50890000000000002</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="34">
         <v>0.48870000000000002</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="34">
         <v>0.49659999999999999</v>
       </c>
-      <c r="M5" s="39">
+      <c r="M5" s="34">
         <v>0.48270000000000002</v>
       </c>
-      <c r="N5" s="39">
+      <c r="N5" s="34">
         <v>0.47439999999999999</v>
       </c>
-      <c r="O5" s="33" t="s">
+      <c r="O5" s="60" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="Q5" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="R5" s="69">
+        <v>65.7</v>
+      </c>
+      <c r="S5" s="69">
+        <v>61.2</v>
+      </c>
+      <c r="T5" s="71">
+        <v>57.4</v>
+      </c>
+      <c r="U5" s="68">
+        <v>72.2</v>
+      </c>
+      <c r="V5" s="71">
+        <v>56.4</v>
+      </c>
+      <c r="W5" s="72">
+        <v>54.4</v>
+      </c>
+      <c r="X5" s="72">
+        <v>53.2</v>
+      </c>
+      <c r="Y5" s="72">
+        <v>51.6</v>
+      </c>
+      <c r="Z5" s="72">
+        <v>50.7</v>
+      </c>
+      <c r="AA5" s="72">
+        <v>50.1</v>
+      </c>
+      <c r="AB5" s="70">
+        <v>49.9</v>
+      </c>
+      <c r="AC5" s="70">
+        <v>49.6</v>
+      </c>
+      <c r="AD5" s="70">
+        <v>49.4</v>
+      </c>
+      <c r="AE5" s="60" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="24">
         <v>0.6321</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="29">
         <v>0.59799999999999998</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="29">
         <v>0.56510000000000005</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>0.54120000000000001</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="26">
         <v>0.75</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="25">
         <v>0.52669999999999995</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="25">
         <v>0.51859999999999995</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="25">
         <v>0.50309999999999999</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="25">
         <v>0.50249999999999995</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="34">
         <v>0.47270000000000001</v>
       </c>
-      <c r="L6" s="39">
+      <c r="L6" s="34">
         <v>0.46700000000000003</v>
       </c>
-      <c r="M6" s="39">
+      <c r="M6" s="34">
         <v>0.45390000000000003</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="23">
         <v>0.4446</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="O6" s="60" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="Q6" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="R6" s="69">
+        <v>65</v>
+      </c>
+      <c r="S6" s="69">
+        <v>60.9</v>
+      </c>
+      <c r="T6" s="71">
+        <v>56.8</v>
+      </c>
+      <c r="U6" s="72">
+        <v>54.2</v>
+      </c>
+      <c r="V6" s="69">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="W6" s="72">
+        <v>52.5</v>
+      </c>
+      <c r="X6" s="72">
+        <v>50.4</v>
+      </c>
+      <c r="Y6" s="70">
+        <v>49.7</v>
+      </c>
+      <c r="Z6" s="70">
+        <v>47.8</v>
+      </c>
+      <c r="AA6" s="70">
+        <v>46.5</v>
+      </c>
+      <c r="AB6" s="70">
+        <v>46.3</v>
+      </c>
+      <c r="AC6" s="70">
+        <v>45.7</v>
+      </c>
+      <c r="AD6" s="70">
+        <v>46</v>
+      </c>
+      <c r="AE6" s="60" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="59">
         <v>9</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="24">
         <v>0.61260000000000003</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="29">
         <v>0.57240000000000002</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="29">
         <v>0.55840000000000001</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>0.53869999999999996</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="25">
         <v>0.51870000000000005</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="26">
         <v>0.72</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="25">
         <v>0.50980000000000003</v>
       </c>
-      <c r="I7" s="40">
+      <c r="I7" s="35">
         <v>0.48120000000000002</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="35">
         <v>0.4844</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="34">
         <v>0.45689999999999997</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="34">
         <v>0.45200000000000001</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="23">
         <v>0.43609999999999999</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="23">
         <v>0.42080000000000001</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="60">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="Q7" s="66">
+        <v>9</v>
+      </c>
+      <c r="R7" s="69">
+        <v>63.7</v>
+      </c>
+      <c r="S7" s="71">
+        <v>59</v>
+      </c>
+      <c r="T7" s="71">
+        <v>55.5</v>
+      </c>
+      <c r="U7" s="72">
+        <v>52.5</v>
+      </c>
+      <c r="V7" s="70">
+        <v>49.5</v>
+      </c>
+      <c r="W7" s="69">
+        <v>65.8</v>
+      </c>
+      <c r="X7" s="70">
+        <v>48.9</v>
+      </c>
+      <c r="Y7" s="70">
+        <v>46.9</v>
+      </c>
+      <c r="Z7" s="70">
+        <v>46</v>
+      </c>
+      <c r="AA7" s="70">
+        <v>44.3</v>
+      </c>
+      <c r="AB7" s="70">
+        <v>42.8</v>
+      </c>
+      <c r="AC7" s="70">
+        <v>42.9</v>
+      </c>
+      <c r="AD7" s="70">
+        <v>42.4</v>
+      </c>
+      <c r="AE7" s="60">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="59">
         <v>8</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="24">
         <v>0.60150000000000003</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="25">
         <v>0.53890000000000005</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="25">
         <v>0.54</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>0.50800000000000001</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="34">
         <v>0.49719999999999998</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="34">
         <v>0.48720000000000002</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="24">
         <v>0.69</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="34">
         <v>0.48970000000000002</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="34">
         <v>0.46550000000000002</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="23">
         <v>0.44440000000000002</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="23">
         <v>0.4264</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="23">
         <v>0.42609999999999998</v>
       </c>
-      <c r="N8" s="22">
+      <c r="N8" s="20">
         <v>0.39250000000000002</v>
       </c>
-      <c r="O8" s="33">
+      <c r="O8" s="60">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="Q8" s="66">
+        <v>8</v>
+      </c>
+      <c r="R8" s="69">
+        <v>63.2</v>
+      </c>
+      <c r="S8" s="71">
+        <v>57.5</v>
+      </c>
+      <c r="T8" s="72">
+        <v>54</v>
+      </c>
+      <c r="U8" s="72">
+        <v>50.8</v>
+      </c>
+      <c r="V8" s="70">
+        <v>48.2</v>
+      </c>
+      <c r="W8" s="70">
+        <v>45.8</v>
+      </c>
+      <c r="X8" s="69">
+        <v>63.2</v>
+      </c>
+      <c r="Y8" s="70">
+        <v>45.1</v>
+      </c>
+      <c r="Z8" s="70">
+        <v>43.8</v>
+      </c>
+      <c r="AA8" s="70">
+        <v>42.4</v>
+      </c>
+      <c r="AB8" s="70">
+        <v>41.1</v>
+      </c>
+      <c r="AC8" s="70">
+        <v>40.1</v>
+      </c>
+      <c r="AD8" s="70">
+        <v>40</v>
+      </c>
+      <c r="AE8" s="60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="59">
         <v>7</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="29">
         <v>0.58789999999999998</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="25">
         <v>0.54520000000000002</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="25">
         <v>0.51670000000000005</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="34">
         <v>0.49580000000000002</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="34">
         <v>0.48630000000000001</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="36">
         <v>0.45429999999999998</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="34">
         <v>0.4501</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="24">
         <v>0.66</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="23">
         <v>0.44590000000000002</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="23">
         <v>0.42949999999999999</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="23">
         <v>0.41260000000000002</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="20">
         <v>0.3952</v>
       </c>
-      <c r="N9" s="22">
+      <c r="N9" s="20">
         <v>0.37359999999999999</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="60">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="Q9" s="66">
+        <v>7</v>
+      </c>
+      <c r="R9" s="69">
+        <v>62.3</v>
+      </c>
+      <c r="S9" s="71">
+        <v>57.3</v>
+      </c>
+      <c r="T9" s="72">
+        <v>52.4</v>
+      </c>
+      <c r="U9" s="70">
+        <v>49.3</v>
+      </c>
+      <c r="V9" s="70">
+        <v>46.7</v>
+      </c>
+      <c r="W9" s="70">
+        <v>43.9</v>
+      </c>
+      <c r="X9" s="70">
+        <v>42.3</v>
+      </c>
+      <c r="Y9" s="69">
+        <v>60.7</v>
+      </c>
+      <c r="Z9" s="70">
+        <v>42.5</v>
+      </c>
+      <c r="AA9" s="70">
+        <v>41.1</v>
+      </c>
+      <c r="AB9" s="70">
+        <v>40</v>
+      </c>
+      <c r="AC9" s="70">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="AD9" s="70">
+        <v>38</v>
+      </c>
+      <c r="AE9" s="60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="59">
         <v>6</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="29">
         <v>0.58050000000000002</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="25">
         <v>0.54730000000000001</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="25">
         <v>0.51590000000000003</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="34">
         <v>0.48770000000000002</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="34">
         <v>0.45660000000000001</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="36">
         <v>0.4572</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="23">
         <v>0.4466</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="23">
         <v>0.42399999999999999</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="24">
         <v>0.64</v>
       </c>
-      <c r="K10" s="41">
+      <c r="K10" s="36">
         <v>0.42470000000000002</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="36">
         <v>0.4284</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="30">
         <v>0.37819999999999998</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="30">
         <v>0.37869999999999998</v>
       </c>
-      <c r="O10" s="33">
+      <c r="O10" s="60">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="Q10" s="66">
+        <v>6</v>
+      </c>
+      <c r="R10" s="69">
+        <v>62</v>
+      </c>
+      <c r="S10" s="71">
+        <v>56.5</v>
+      </c>
+      <c r="T10" s="72">
+        <v>51.9</v>
+      </c>
+      <c r="U10" s="70">
+        <v>47.7</v>
+      </c>
+      <c r="V10" s="70">
+        <v>45</v>
+      </c>
+      <c r="W10" s="70">
+        <v>42.8</v>
+      </c>
+      <c r="X10" s="70">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="Y10" s="70">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="Z10" s="71">
+        <v>58.7</v>
+      </c>
+      <c r="AA10" s="70">
+        <v>40</v>
+      </c>
+      <c r="AB10" s="70">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="AC10" s="70">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="AD10" s="70">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="AE10" s="60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="59">
         <v>5</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="29">
         <v>0.58720000000000006</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="25">
         <v>0.53510000000000002</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="25">
         <v>0.50329999999999997</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="34">
         <v>0.4632</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="23">
         <v>0.43830000000000002</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G11" s="36">
         <v>0.4178</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="23">
         <v>0.41699999999999998</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="23">
         <v>0.41099999999999998</v>
       </c>
-      <c r="J11" s="41">
+      <c r="J11" s="36">
         <v>0.39950000000000002</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="24">
         <v>0.6</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="36">
         <v>0.4209</v>
       </c>
-      <c r="M11" s="41">
+      <c r="M11" s="36">
         <v>0.40089999999999998</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="20">
         <v>0.37169999999999997</v>
       </c>
-      <c r="O11" s="33">
+      <c r="O11" s="60">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="Q11" s="66">
+        <v>5</v>
+      </c>
+      <c r="R11" s="69">
+        <v>61.4</v>
+      </c>
+      <c r="S11" s="71">
+        <v>55.9</v>
+      </c>
+      <c r="T11" s="72">
+        <v>51.3</v>
+      </c>
+      <c r="U11" s="70">
+        <v>47.4</v>
+      </c>
+      <c r="V11" s="70">
+        <v>43.5</v>
+      </c>
+      <c r="W11" s="70">
+        <v>41.3</v>
+      </c>
+      <c r="X11" s="70">
+        <v>39.1</v>
+      </c>
+      <c r="Y11" s="70">
+        <v>37.6</v>
+      </c>
+      <c r="Z11" s="70">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="AA11" s="71">
+        <v>56.6</v>
+      </c>
+      <c r="AB11" s="70">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="AC11" s="70">
+        <v>36.4</v>
+      </c>
+      <c r="AD11" s="70">
+        <v>35.6</v>
+      </c>
+      <c r="AE11" s="60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59">
         <v>4</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="29">
         <v>0.55740000000000001</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="25">
         <v>0.52339999999999998</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="34">
         <v>0.496</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="34">
         <v>0.45750000000000002</v>
       </c>
-      <c r="F12" s="41">
+      <c r="F12" s="36">
         <v>0.42459999999999998</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="36">
         <v>0.4219</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="20">
         <v>0.39489999999999997</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="20">
         <v>0.38390000000000002</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J12" s="36">
         <v>0.4</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="20">
         <v>0.38069999999999998</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="22">
         <v>0.56999999999999995</v>
       </c>
-      <c r="M12" s="32">
+      <c r="M12" s="30">
         <v>0.38890000000000002</v>
       </c>
-      <c r="N12" s="32">
+      <c r="N12" s="30">
         <v>0.38109999999999999</v>
       </c>
-      <c r="O12" s="33">
+      <c r="O12" s="60">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="Q12" s="66">
+        <v>4</v>
+      </c>
+      <c r="R12" s="69">
+        <v>61</v>
+      </c>
+      <c r="S12" s="71">
+        <v>55.5</v>
+      </c>
+      <c r="T12" s="72">
+        <v>50.9</v>
+      </c>
+      <c r="U12" s="70">
+        <v>47</v>
+      </c>
+      <c r="V12" s="70">
+        <v>43.1</v>
+      </c>
+      <c r="W12" s="70">
+        <v>39.6</v>
+      </c>
+      <c r="X12" s="70">
+        <v>38</v>
+      </c>
+      <c r="Y12" s="70">
+        <v>36.5</v>
+      </c>
+      <c r="Z12" s="70">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="AA12" s="70">
+        <v>34</v>
+      </c>
+      <c r="AB12" s="72">
+        <v>54.6</v>
+      </c>
+      <c r="AC12" s="70">
+        <v>35.9</v>
+      </c>
+      <c r="AD12" s="70">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="AE12" s="60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="59">
         <v>3</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="29">
         <v>0.56079999999999997</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="25">
         <v>0.5151</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="34">
         <v>0.47560000000000002</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="34">
         <v>0.4612</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="36">
         <v>0.42849999999999999</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="23">
         <v>0.40400000000000003</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="20">
         <v>0.37380000000000002</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="20">
         <v>0.36959999999999998</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="20">
         <v>0.35799999999999998</v>
       </c>
-      <c r="K13" s="32">
+      <c r="K13" s="30">
         <v>0.3493</v>
       </c>
-      <c r="L13" s="32">
+      <c r="L13" s="30">
         <v>0.35649999999999998</v>
       </c>
-      <c r="M13" s="27">
+      <c r="M13" s="25">
         <v>0.53</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="30">
         <v>0.36670000000000003</v>
       </c>
-      <c r="O13" s="33">
+      <c r="O13" s="60">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="Q13" s="66">
+        <v>3</v>
+      </c>
+      <c r="R13" s="69">
+        <v>60.5</v>
+      </c>
+      <c r="S13" s="71">
+        <v>55.5</v>
+      </c>
+      <c r="T13" s="72">
+        <v>50.9</v>
+      </c>
+      <c r="U13" s="70">
+        <v>46.7</v>
+      </c>
+      <c r="V13" s="70">
+        <v>42.8</v>
+      </c>
+      <c r="W13" s="70">
+        <v>39.6</v>
+      </c>
+      <c r="X13" s="70">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="Y13" s="70">
+        <v>35.1</v>
+      </c>
+      <c r="Z13" s="70">
+        <v>34</v>
+      </c>
+      <c r="AA13" s="70">
+        <v>32.9</v>
+      </c>
+      <c r="AB13" s="70">
+        <v>31.9</v>
+      </c>
+      <c r="AC13" s="72">
+        <v>52.6</v>
+      </c>
+      <c r="AD13" s="70">
+        <v>34.4</v>
+      </c>
+      <c r="AE13" s="60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="59">
         <v>2</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="29">
         <v>0.55730000000000002</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="25">
         <v>0.5242</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="34">
         <v>0.47260000000000002</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="23">
         <v>0.439</v>
       </c>
-      <c r="F14" s="41">
+      <c r="F14" s="36">
         <v>0.42659999999999998</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="20">
         <v>0.39789999999999998</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="20">
         <v>0.36380000000000001</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="20">
         <v>0.35249999999999998</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="20">
         <v>0.34150000000000003</v>
       </c>
-      <c r="K14" s="32">
+      <c r="K14" s="30">
         <v>0.33810000000000001</v>
       </c>
-      <c r="L14" s="32">
+      <c r="L14" s="30">
         <v>0.34889999999999999</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="20">
         <v>0.32379999999999998</v>
       </c>
-      <c r="N14" s="27">
+      <c r="N14" s="25">
         <v>0.5</v>
       </c>
-      <c r="O14" s="33">
+      <c r="O14" s="60">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" s="38" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35" t="s">
+      <c r="Q14" s="66">
+        <v>2</v>
+      </c>
+      <c r="R14" s="69">
+        <v>60.7</v>
+      </c>
+      <c r="S14" s="71">
+        <v>55.4</v>
+      </c>
+      <c r="T14" s="72">
+        <v>50.7</v>
+      </c>
+      <c r="U14" s="70">
+        <v>46.7</v>
+      </c>
+      <c r="V14" s="70">
+        <v>42.6</v>
+      </c>
+      <c r="W14" s="70">
+        <v>39.4</v>
+      </c>
+      <c r="X14" s="70">
+        <v>36.6</v>
+      </c>
+      <c r="Y14" s="70">
+        <v>34.5</v>
+      </c>
+      <c r="Z14" s="70">
+        <v>33</v>
+      </c>
+      <c r="AA14" s="70">
+        <v>31.8</v>
+      </c>
+      <c r="AB14" s="70">
+        <v>30.9</v>
+      </c>
+      <c r="AC14" s="70">
+        <v>30.5</v>
+      </c>
+      <c r="AD14" s="72">
+        <v>50.8</v>
+      </c>
+      <c r="AE14" s="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" s="33" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="63">
         <v>9</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="63">
         <v>8</v>
       </c>
-      <c r="I15" s="36">
+      <c r="I15" s="63">
         <v>7</v>
       </c>
-      <c r="J15" s="36">
+      <c r="J15" s="63">
         <v>6</v>
       </c>
-      <c r="K15" s="36">
+      <c r="K15" s="63">
         <v>5</v>
       </c>
-      <c r="L15" s="36">
+      <c r="L15" s="63">
         <v>4</v>
       </c>
-      <c r="M15" s="36">
+      <c r="M15" s="63">
         <v>3</v>
       </c>
-      <c r="N15" s="36">
+      <c r="N15" s="63">
         <v>2</v>
       </c>
-      <c r="O15" s="37"/>
-    </row>
-    <row r="16" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="28">
+      <c r="O15" s="32"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="S15" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="T15" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="U15" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="V15" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="W15" s="63">
+        <v>9</v>
+      </c>
+      <c r="X15" s="63">
+        <v>8</v>
+      </c>
+      <c r="Y15" s="63">
+        <v>7</v>
+      </c>
+      <c r="Z15" s="63">
+        <v>6</v>
+      </c>
+      <c r="AA15" s="63">
+        <v>5</v>
+      </c>
+      <c r="AB15" s="63">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="63">
+        <v>3</v>
+      </c>
+      <c r="AD15" s="63">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="64"/>
+    </row>
+    <row r="16" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="26">
         <v>0.7</v>
       </c>
       <c r="D16" t="s">
         <v>154</v>
       </c>
-      <c r="F16" s="30"/>
+      <c r="F16" s="28"/>
       <c r="G16" t="s">
         <v>152</v>
       </c>
-      <c r="I16" s="29"/>
+      <c r="I16" s="27"/>
       <c r="J16" t="s">
         <v>151</v>
       </c>
-      <c r="L16" s="27"/>
+      <c r="L16" s="25"/>
       <c r="M16" t="s">
         <v>153</v>
+      </c>
+      <c r="S16" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="T16" t="s">
+        <v>154</v>
+      </c>
+      <c r="V16" s="28"/>
+      <c r="W16" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y16" s="71"/>
+      <c r="Z16" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB16" s="72"/>
+      <c r="AC16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D18" s="65" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="U18" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="V18" s="65"/>
+      <c r="W18" s="65"/>
+      <c r="X18" s="65"/>
+      <c r="Y18" s="65"/>
+      <c r="Z18" s="65"/>
+      <c r="AA18" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="U18:AA18"/>
+    <mergeCell ref="D18:K18"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="A1:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" style="11" customWidth="1"/>
+    <col min="2" max="14" width="5.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="54" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="54">
+        <v>9</v>
+      </c>
+      <c r="H1" s="54">
+        <v>8</v>
+      </c>
+      <c r="I1" s="54">
+        <v>7</v>
+      </c>
+      <c r="J1" s="54">
+        <v>6</v>
+      </c>
+      <c r="K1" s="54">
+        <v>5</v>
+      </c>
+      <c r="L1" s="54">
+        <v>4</v>
+      </c>
+      <c r="M1" s="54">
+        <v>3</v>
+      </c>
+      <c r="N1" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2">
+        <v>85.9</v>
+      </c>
+      <c r="C2">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="D2">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="E2">
+        <v>67.5</v>
+      </c>
+      <c r="F2">
+        <v>67.2</v>
+      </c>
+      <c r="G2">
+        <v>65.8</v>
+      </c>
+      <c r="H2">
+        <v>65</v>
+      </c>
+      <c r="I2">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="J2">
+        <v>63.9</v>
+      </c>
+      <c r="K2">
+        <v>63.4</v>
+      </c>
+      <c r="L2">
+        <v>63.3</v>
+      </c>
+      <c r="M2">
+        <v>63.2</v>
+      </c>
+      <c r="N2">
+        <v>62.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="C3">
+        <v>80.8</v>
+      </c>
+      <c r="D3">
+        <v>63.7</v>
+      </c>
+      <c r="E3">
+        <v>63.3</v>
+      </c>
+      <c r="F3">
+        <v>63</v>
+      </c>
+      <c r="G3">
+        <v>61.7</v>
+      </c>
+      <c r="H3">
+        <v>59.8</v>
+      </c>
+      <c r="I3">
+        <v>59.9</v>
+      </c>
+      <c r="J3">
+        <v>59.1</v>
+      </c>
+      <c r="K3">
+        <v>58.1</v>
+      </c>
+      <c r="L3">
+        <v>57.8</v>
+      </c>
+      <c r="M3">
+        <v>57.8</v>
+      </c>
+      <c r="N3">
+        <v>58.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="C4">
+        <v>61.9</v>
+      </c>
+      <c r="D4">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="E4">
+        <v>59.6</v>
+      </c>
+      <c r="F4">
+        <v>59.4</v>
+      </c>
+      <c r="G4">
+        <v>57.6</v>
+      </c>
+      <c r="H4">
+        <v>56</v>
+      </c>
+      <c r="I4">
+        <v>55.1</v>
+      </c>
+      <c r="J4">
+        <v>54.2</v>
+      </c>
+      <c r="K4">
+        <v>54.2</v>
+      </c>
+      <c r="L4">
+        <v>53.9</v>
+      </c>
+      <c r="M4">
+        <v>53.3</v>
+      </c>
+      <c r="N4">
+        <v>53.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="C5">
+        <v>61.1</v>
+      </c>
+      <c r="D5">
+        <v>57.6</v>
+      </c>
+      <c r="E5">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="F5">
+        <v>56.4</v>
+      </c>
+      <c r="G5">
+        <v>54.7</v>
+      </c>
+      <c r="H5">
+        <v>53.5</v>
+      </c>
+      <c r="I5">
+        <v>51.9</v>
+      </c>
+      <c r="J5">
+        <v>50.2</v>
+      </c>
+      <c r="K5">
+        <v>50.1</v>
+      </c>
+      <c r="L5">
+        <v>49.8</v>
+      </c>
+      <c r="M5">
+        <v>49.3</v>
+      </c>
+      <c r="N5">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6">
+        <v>65.3</v>
+      </c>
+      <c r="C6">
+        <v>61.2</v>
+      </c>
+      <c r="D6">
+        <v>57.3</v>
+      </c>
+      <c r="E6">
+        <v>54</v>
+      </c>
+      <c r="F6">
+        <v>69</v>
+      </c>
+      <c r="G6">
+        <v>51.9</v>
+      </c>
+      <c r="H6">
+        <v>51.2</v>
+      </c>
+      <c r="I6">
+        <v>49.6</v>
+      </c>
+      <c r="J6">
+        <v>47.9</v>
+      </c>
+      <c r="K6">
+        <v>46.5</v>
+      </c>
+      <c r="L6">
+        <v>46.3</v>
+      </c>
+      <c r="M6">
+        <v>46.1</v>
+      </c>
+      <c r="N6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>62.9</v>
+      </c>
+      <c r="C7">
+        <v>59.4</v>
+      </c>
+      <c r="D7">
+        <v>55.5</v>
+      </c>
+      <c r="E7">
+        <v>52.2</v>
+      </c>
+      <c r="F7">
+        <v>49.7</v>
+      </c>
+      <c r="G7">
+        <v>65.7</v>
+      </c>
+      <c r="H7">
+        <v>48.5</v>
+      </c>
+      <c r="I7">
+        <v>47.1</v>
+      </c>
+      <c r="J7">
+        <v>45.7</v>
+      </c>
+      <c r="K7">
+        <v>44.3</v>
+      </c>
+      <c r="L7">
+        <v>42.4</v>
+      </c>
+      <c r="M7">
+        <v>42.9</v>
+      </c>
+      <c r="N7">
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>63.3</v>
+      </c>
+      <c r="C8">
+        <v>57.8</v>
+      </c>
+      <c r="D8">
+        <v>54</v>
+      </c>
+      <c r="E8">
+        <v>50.7</v>
+      </c>
+      <c r="F8">
+        <v>48.1</v>
+      </c>
+      <c r="G8">
+        <v>45.8</v>
+      </c>
+      <c r="H8">
+        <v>63.2</v>
+      </c>
+      <c r="I8">
+        <v>45.3</v>
+      </c>
+      <c r="J8">
+        <v>43.8</v>
+      </c>
+      <c r="K8">
+        <v>42.4</v>
+      </c>
+      <c r="L8">
+        <v>41.1</v>
+      </c>
+      <c r="M8">
+        <v>40.1</v>
+      </c>
+      <c r="N8">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>62.5</v>
+      </c>
+      <c r="C9">
+        <v>57.4</v>
+      </c>
+      <c r="D9">
+        <v>52.6</v>
+      </c>
+      <c r="E9">
+        <v>49.1</v>
+      </c>
+      <c r="F9">
+        <v>46.6</v>
+      </c>
+      <c r="G9">
+        <v>44.3</v>
+      </c>
+      <c r="H9">
+        <v>42.4</v>
+      </c>
+      <c r="I9">
+        <v>60.6</v>
+      </c>
+      <c r="J9">
+        <v>42.9</v>
+      </c>
+      <c r="K9">
+        <v>41</v>
+      </c>
+      <c r="L9">
+        <v>39.9</v>
+      </c>
+      <c r="M9">
+        <v>38.4</v>
+      </c>
+      <c r="N9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>61.7</v>
+      </c>
+      <c r="C10">
+        <v>56.8</v>
+      </c>
+      <c r="D10">
+        <v>52.1</v>
+      </c>
+      <c r="E10">
+        <v>47.7</v>
+      </c>
+      <c r="F10">
+        <v>44.9</v>
+      </c>
+      <c r="G10">
+        <v>42.9</v>
+      </c>
+      <c r="H10">
+        <v>41.1</v>
+      </c>
+      <c r="I10">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="J10">
+        <v>58.7</v>
+      </c>
+      <c r="K10">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="L10">
+        <v>38.9</v>
+      </c>
+      <c r="M10">
+        <v>37.6</v>
+      </c>
+      <c r="N10">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>61.2</v>
+      </c>
+      <c r="C11">
+        <v>56.2</v>
+      </c>
+      <c r="D11">
+        <v>51.1</v>
+      </c>
+      <c r="E11">
+        <v>47.5</v>
+      </c>
+      <c r="F11">
+        <v>43.5</v>
+      </c>
+      <c r="G11">
+        <v>41.5</v>
+      </c>
+      <c r="H11">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="I11">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="J11">
+        <v>36.6</v>
+      </c>
+      <c r="K11">
+        <v>56.5</v>
+      </c>
+      <c r="L11">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="M11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="N11">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>61.2</v>
+      </c>
+      <c r="C12">
+        <v>55.8</v>
+      </c>
+      <c r="D12">
+        <v>50.9</v>
+      </c>
+      <c r="E12">
+        <v>46.9</v>
+      </c>
+      <c r="F12">
+        <v>43.1</v>
+      </c>
+      <c r="G12">
+        <v>39.9</v>
+      </c>
+      <c r="H12">
+        <v>37.9</v>
+      </c>
+      <c r="I12">
+        <v>36.5</v>
+      </c>
+      <c r="J12">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="K12">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="L12">
+        <v>54.2</v>
+      </c>
+      <c r="M12">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="N12">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>60.8</v>
+      </c>
+      <c r="C13">
+        <v>55.7</v>
+      </c>
+      <c r="D13">
+        <v>51.1</v>
+      </c>
+      <c r="E13">
+        <v>47</v>
+      </c>
+      <c r="F13">
+        <v>43</v>
+      </c>
+      <c r="G13">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="H13">
+        <v>36.5</v>
+      </c>
+      <c r="I13">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="J13">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="K13">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="L13">
+        <v>32.4</v>
+      </c>
+      <c r="M13">
+        <v>52.9</v>
+      </c>
+      <c r="N13">
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>60.6</v>
+      </c>
+      <c r="C14">
+        <v>55.3</v>
+      </c>
+      <c r="D14">
+        <v>50.5</v>
+      </c>
+      <c r="E14">
+        <v>46.8</v>
+      </c>
+      <c r="F14">
+        <v>42.8</v>
+      </c>
+      <c r="G14">
+        <v>39.5</v>
+      </c>
+      <c r="H14">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="I14">
+        <v>34.1</v>
+      </c>
+      <c r="J14">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="K14">
+        <v>31.8</v>
+      </c>
+      <c r="L14">
+        <v>31.4</v>
+      </c>
+      <c r="M14">
+        <v>30.6</v>
+      </c>
+      <c r="N14">
+        <v>51.1</v>
       </c>
     </row>
   </sheetData>
@@ -4048,461 +5469,461 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H1" sqref="H1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="4.125" style="46"/>
+    <col min="1" max="7" width="4.125" style="41"/>
     <col min="8" max="8" width="16.375" style="3" customWidth="1"/>
     <col min="9" max="16384" width="4.125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="47">
+      <c r="A1" s="42">
         <v>4</v>
       </c>
-      <c r="B1" s="47">
+      <c r="B1" s="42">
         <v>3</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="55" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="51" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="47">
+      <c r="A2" s="52">
         <v>4</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="52">
         <v>2</v>
       </c>
-      <c r="C2" s="50">
+      <c r="C2" s="53">
         <v>1</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="55"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="47">
+      <c r="A3" s="42">
         <v>4</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="42">
         <v>1</v>
       </c>
-      <c r="C3" s="50">
+      <c r="C3" s="45">
         <v>1</v>
       </c>
-      <c r="D3" s="50">
+      <c r="D3" s="45">
         <v>1</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="55"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="51"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="47">
+      <c r="A4" s="42">
         <v>3</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="42">
         <v>3</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="45">
         <v>1</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="55"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="51"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="47">
+      <c r="A5" s="42">
         <v>3</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="42">
         <v>2</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="45">
         <v>2</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="55"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="51"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="47">
+      <c r="A6" s="42">
         <v>3</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="42">
         <v>2</v>
       </c>
-      <c r="C6" s="50">
+      <c r="C6" s="45">
         <v>1</v>
       </c>
-      <c r="D6" s="50">
+      <c r="D6" s="45">
         <v>1</v>
       </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="55"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="51"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="53">
+      <c r="A7" s="48">
         <v>3</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="48">
         <v>1</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="47">
         <v>1</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="47">
         <v>1</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="47">
         <v>1</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="55"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="51"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="47">
+      <c r="A8" s="42">
         <v>2</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="42">
         <v>2</v>
       </c>
-      <c r="C8" s="50">
+      <c r="C8" s="45">
         <v>2</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="45">
         <v>1</v>
       </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="55"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="51"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="53">
+      <c r="A9" s="48">
         <v>2</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="48">
         <v>2</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="49">
         <v>1</v>
       </c>
-      <c r="D9" s="52">
+      <c r="D9" s="47">
         <v>1</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="47">
         <v>1</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="55"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="51"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="53">
+      <c r="A10" s="48">
         <v>2</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="48">
         <v>1</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="49">
         <v>1</v>
       </c>
-      <c r="D10" s="52">
+      <c r="D10" s="47">
         <v>1</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="47">
         <v>1</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="47">
         <v>1</v>
       </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="55"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="51"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="51">
+      <c r="A11" s="46">
         <v>1</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B11" s="46">
         <v>1</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="47">
         <v>1</v>
       </c>
-      <c r="D11" s="52">
+      <c r="D11" s="47">
         <v>1</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="47">
         <v>1</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F11" s="47">
         <v>1</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="47">
         <v>1</v>
       </c>
-      <c r="H11" s="55"/>
+      <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="49"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="50">
+      <c r="A19" s="45">
         <v>7</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="55" t="s">
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="51" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="50">
+      <c r="A20" s="45">
         <v>6</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="44">
         <v>1</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="55"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="51"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="50">
+      <c r="A21" s="45">
         <v>5</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="44">
         <v>2</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="55"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="51"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="50">
+      <c r="A22" s="45">
         <v>5</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="44">
         <v>1</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="44">
         <v>1</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="55"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="51"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="49">
+      <c r="A23" s="44">
         <v>4</v>
       </c>
-      <c r="B23" s="49">
+      <c r="B23" s="44">
         <v>3</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="55"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="51"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="49">
+      <c r="A24" s="44">
         <v>4</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="44">
         <v>2</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="44">
         <v>1</v>
       </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="55"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="51"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="49">
+      <c r="A25" s="44">
         <v>4</v>
       </c>
-      <c r="B25" s="49">
+      <c r="B25" s="44">
         <v>1</v>
       </c>
-      <c r="C25" s="49">
+      <c r="C25" s="44">
         <v>1</v>
       </c>
-      <c r="D25" s="49">
+      <c r="D25" s="44">
         <v>1</v>
       </c>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="55"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="49">
+      <c r="A26" s="44">
         <v>3</v>
       </c>
-      <c r="B26" s="49">
+      <c r="B26" s="44">
         <v>3</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="44">
         <v>1</v>
       </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="55"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="51"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="49">
+      <c r="A27" s="44">
         <v>3</v>
       </c>
-      <c r="B27" s="49">
+      <c r="B27" s="44">
         <v>2</v>
       </c>
-      <c r="C27" s="49">
+      <c r="C27" s="44">
         <v>2</v>
       </c>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="55"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="51"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="49">
+      <c r="A28" s="44">
         <v>3</v>
       </c>
-      <c r="B28" s="49">
+      <c r="B28" s="44">
         <v>2</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="44">
         <v>1</v>
       </c>
-      <c r="D28" s="49">
+      <c r="D28" s="44">
         <v>1</v>
       </c>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="55"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="51"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="49">
+      <c r="A29" s="44">
         <v>2</v>
       </c>
-      <c r="B29" s="49">
+      <c r="B29" s="44">
         <v>2</v>
       </c>
-      <c r="C29" s="49">
+      <c r="C29" s="44">
         <v>2</v>
       </c>
-      <c r="D29" s="49">
+      <c r="D29" s="44">
         <v>1</v>
       </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="55"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4515,7 +5936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O52"/>
   <sheetViews>
@@ -4529,69 +5950,69 @@
     <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7.5" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="4.5" style="56" customWidth="1"/>
+    <col min="10" max="10" width="4.5" style="50" customWidth="1"/>
     <col min="11" max="11" width="3.5" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="30">
+      <c r="A1" s="28">
         <v>249900</v>
       </c>
-      <c r="B1" s="30">
+      <c r="B1" s="28">
         <v>0</v>
       </c>
-      <c r="C1" s="30">
+      <c r="C1" s="28">
         <v>0</v>
       </c>
-      <c r="D1" s="30">
+      <c r="D1" s="28">
         <v>0</v>
       </c>
-      <c r="E1" s="30">
+      <c r="E1" s="28">
         <v>0</v>
       </c>
-      <c r="F1" s="30">
+      <c r="F1" s="28">
         <v>1</v>
       </c>
-      <c r="G1" s="30">
+      <c r="G1" s="28">
         <v>2</v>
       </c>
-      <c r="H1" s="30">
+      <c r="H1" s="28">
         <v>3</v>
       </c>
-      <c r="I1" s="30">
+      <c r="I1" s="28">
         <v>4</v>
       </c>
-      <c r="J1" s="30">
+      <c r="J1" s="28">
         <v>48</v>
       </c>
-      <c r="L1" s="30">
+      <c r="L1" s="28">
         <v>1</v>
       </c>
-      <c r="M1" s="30">
+      <c r="M1" s="28">
         <v>2</v>
       </c>
-      <c r="N1" s="30">
+      <c r="N1" s="28">
         <v>3</v>
       </c>
-      <c r="O1" s="30">
+      <c r="O1" s="28">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="30">
+      <c r="A2" s="28">
         <v>230300</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="40">
         <v>19600</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="28">
         <v>0</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="28">
         <v>0</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="28">
         <v>0</v>
       </c>
       <c r="I2">
@@ -4614,19 +6035,19 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="30">
+      <c r="A3" s="28">
         <v>211876</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="28">
         <v>36848</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="28">
         <v>1176</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="28">
         <v>0</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="28">
         <v>0</v>
       </c>
       <c r="I3">
@@ -4635,45 +6056,45 @@
       <c r="J3">
         <v>46</v>
       </c>
-      <c r="L3" s="30">
+      <c r="L3" s="28">
         <v>1</v>
       </c>
-      <c r="M3" s="30">
+      <c r="M3" s="28">
         <v>4</v>
       </c>
-      <c r="N3" s="30">
+      <c r="N3" s="28">
         <v>5</v>
       </c>
-      <c r="O3" s="30">
+      <c r="O3" s="28">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="30">
+      <c r="A4" s="28">
         <v>194580</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="28">
         <v>51888</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="28">
         <v>3384</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="28">
         <v>48</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="28">
         <v>0</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="28">
         <v>7</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="28">
         <v>45</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="28">
         <v>5</v>
       </c>
       <c r="N4">
@@ -4684,62 +6105,62 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="30">
+      <c r="A5" s="28">
         <v>178365</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="28">
         <v>64860</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="28">
         <v>6486</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="28">
         <v>188</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="28">
         <v>1</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
       <c r="I5">
         <v>8</v>
       </c>
       <c r="J5">
         <v>44</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="28">
         <v>1</v>
       </c>
       <c r="M5">
         <v>6</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="28">
         <v>7</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="28">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="30">
+      <c r="A6" s="28">
         <v>163185</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="28">
         <v>75900</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="28">
         <v>10350</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="28">
         <v>460</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <v>5</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
       <c r="I6">
         <v>9</v>
       </c>
@@ -4749,7 +6170,7 @@
       <c r="L6">
         <v>1</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="28">
         <v>7</v>
       </c>
       <c r="N6">
@@ -4760,62 +6181,62 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="30">
+      <c r="A7" s="28">
         <v>148995</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="28">
         <v>85140</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="28">
         <v>14850</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="28">
         <v>900</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="28">
         <v>15</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="30">
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="28">
         <v>10</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="28">
         <v>42</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="28">
         <v>1</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M7" s="28">
         <v>8</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="28">
         <v>9</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="28">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="30">
+      <c r="A8" s="28">
         <v>135751</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="28">
         <v>92708</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="28">
         <v>19866</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="28">
         <v>1540</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="28">
         <v>35</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
       <c r="I8">
         <v>11</v>
       </c>
@@ -4836,24 +6257,24 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="30">
+      <c r="A9" s="28">
         <v>123410</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="28">
         <v>98728</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="28">
         <v>25284</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="28">
         <v>2408</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="28">
         <v>70</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
       <c r="I9">
         <v>12</v>
       </c>
@@ -4862,45 +6283,45 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="30">
+      <c r="A10" s="28">
         <v>111930</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="28">
         <v>103320</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="28">
         <v>30996</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="28">
         <v>3528</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="28">
         <v>126</v>
       </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="30">
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="28">
         <v>13</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="28">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30">
+    <row r="11" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="28">
         <v>101270</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="28">
         <v>106600</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="28">
         <v>36900</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="28">
         <v>4920</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="28">
         <v>210</v>
       </c>
       <c r="I11">
@@ -4910,20 +6331,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30">
+    <row r="12" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="28">
         <v>91390</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="28">
         <v>108680</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="28">
         <v>42900</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="28">
         <v>6600</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="28">
         <v>330</v>
       </c>
       <c r="I12">
@@ -4933,43 +6354,43 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="30">
+    <row r="13" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28">
         <v>82251</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="39">
         <v>109668</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="28">
         <v>48906</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="28">
         <v>8580</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="28">
         <v>495</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="28">
         <v>16</v>
       </c>
-      <c r="J13" s="30">
+      <c r="J13" s="28">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30">
+    <row r="14" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="28">
         <v>73815</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="39">
         <v>109668</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="28">
         <v>54834</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="28">
         <v>10868</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="28">
         <v>715</v>
       </c>
       <c r="I14">
@@ -4979,20 +6400,20 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30">
+    <row r="15" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="28">
         <v>66045</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="28">
         <v>108780</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="28">
         <v>60606</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="28">
         <v>13468</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="28">
         <v>1001</v>
       </c>
       <c r="I15">
@@ -5002,43 +6423,43 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="30">
+    <row r="16" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="28">
         <v>58905</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="28">
         <v>107100</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="28">
         <v>66150</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="28">
         <v>16380</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="28">
         <v>1365</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="28">
         <v>19</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J16" s="28">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="30">
+    <row r="17" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="28">
         <v>52360</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="28">
         <v>104720</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="28">
         <v>71400</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="40">
         <v>19600</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="28">
         <v>1820</v>
       </c>
       <c r="F17"/>
@@ -5051,20 +6472,20 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30">
+    <row r="18" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="28">
         <v>46376</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="28">
         <v>101728</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="28">
         <v>76296</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="28">
         <v>23120</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="28">
         <v>2380</v>
       </c>
       <c r="F18"/>
@@ -5077,46 +6498,46 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30">
+    <row r="19" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="28">
         <v>40920</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="28">
         <v>98208</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="28">
         <v>80784</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="28">
         <v>26928</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="28">
         <v>3060</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
-      <c r="I19" s="30">
+      <c r="I19" s="28">
         <v>22</v>
       </c>
-      <c r="J19" s="30">
+      <c r="J19" s="28">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30">
+    <row r="20" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="28">
         <v>35960</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="28">
         <v>94240</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="28">
         <v>84816</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="28">
         <v>31008</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>3876</v>
       </c>
       <c r="F20"/>
@@ -5129,20 +6550,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="30">
+    <row r="21" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="28">
         <v>31465</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="28">
         <v>89900</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="28">
         <v>88350</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="28">
         <v>35340</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="28">
         <v>4845</v>
       </c>
       <c r="F21"/>
@@ -5155,55 +6576,55 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="30">
+    <row r="22" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="28">
         <v>27405</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="28">
         <v>85260</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="28">
         <v>91350</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="28">
         <v>39900</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="28">
         <v>5985</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
-      <c r="I22" s="30">
+      <c r="I22" s="28">
         <v>25</v>
       </c>
-      <c r="J22" s="30">
+      <c r="J22" s="28">
         <v>27</v>
       </c>
-      <c r="L22" s="30">
+      <c r="L22" s="28">
         <v>1</v>
       </c>
-      <c r="M22" s="30">
+      <c r="M22" s="28">
         <v>48</v>
       </c>
-      <c r="N22" s="30">
+      <c r="N22" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="30">
+      <c r="A23" s="28">
         <v>23751</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="28">
         <v>80388</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="28">
         <v>93786</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="28">
         <v>44660</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="28">
         <v>7315</v>
       </c>
       <c r="I23">
@@ -5223,19 +6644,19 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="30">
+      <c r="A24" s="28">
         <v>20475</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B24" s="28">
         <v>75348</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="28">
         <v>95634</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="28">
         <v>49588</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="28">
         <v>8855</v>
       </c>
       <c r="I24">
@@ -5244,36 +6665,36 @@
       <c r="J24">
         <v>25</v>
       </c>
-      <c r="L24" s="30">
+      <c r="L24" s="28">
         <v>3</v>
       </c>
-      <c r="M24" s="30">
+      <c r="M24" s="28">
         <v>46</v>
       </c>
-      <c r="N24" s="30">
+      <c r="N24" s="28">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="30">
+      <c r="A25" s="28">
         <v>17550</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25" s="28">
         <v>70200</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="28">
         <v>96876</v>
       </c>
-      <c r="D25" s="30">
+      <c r="D25" s="28">
         <v>54648</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="28">
         <v>10626</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I25" s="28">
         <v>28</v>
       </c>
-      <c r="J25" s="30">
+      <c r="J25" s="28">
         <v>24</v>
       </c>
       <c r="L25">
@@ -5287,19 +6708,19 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="30">
+      <c r="A26" s="28">
         <v>14950</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="28">
         <v>65000</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="28">
         <v>97500</v>
       </c>
-      <c r="D26" s="30">
+      <c r="D26" s="28">
         <v>59800</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="28">
         <v>12650</v>
       </c>
       <c r="I26">
@@ -5308,30 +6729,30 @@
       <c r="J26">
         <v>23</v>
       </c>
-      <c r="L26" s="30">
+      <c r="L26" s="28">
         <v>5</v>
       </c>
-      <c r="M26" s="30">
+      <c r="M26" s="28">
         <v>44</v>
       </c>
-      <c r="N26" s="30">
+      <c r="N26" s="28">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="43">
+      <c r="A27" s="38">
         <v>12650</v>
       </c>
-      <c r="B27" s="43">
+      <c r="B27" s="38">
         <v>59800</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="38">
         <v>97500</v>
       </c>
-      <c r="D27" s="43">
+      <c r="D27" s="38">
         <v>65000</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="38">
         <v>14950</v>
       </c>
       <c r="I27">
@@ -5351,51 +6772,51 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="43">
+      <c r="A28" s="38">
         <v>10626</v>
       </c>
-      <c r="B28" s="43">
+      <c r="B28" s="38">
         <v>54648</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="38">
         <v>96876</v>
       </c>
-      <c r="D28" s="43">
+      <c r="D28" s="38">
         <v>70200</v>
       </c>
-      <c r="E28" s="43">
+      <c r="E28" s="38">
         <v>17550</v>
       </c>
-      <c r="I28" s="30">
+      <c r="I28" s="28">
         <v>31</v>
       </c>
-      <c r="J28" s="30">
+      <c r="J28" s="28">
         <v>21</v>
       </c>
-      <c r="L28" s="30">
+      <c r="L28" s="28">
         <v>7</v>
       </c>
-      <c r="M28" s="30">
+      <c r="M28" s="28">
         <v>42</v>
       </c>
-      <c r="N28" s="30">
+      <c r="N28" s="28">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="43">
+      <c r="A29" s="38">
         <v>8855</v>
       </c>
-      <c r="B29" s="43">
+      <c r="B29" s="38">
         <v>49588</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="38">
         <v>95634</v>
       </c>
-      <c r="D29" s="43">
+      <c r="D29" s="38">
         <v>75348</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="38">
         <v>20475</v>
       </c>
       <c r="I29">
@@ -5415,19 +6836,19 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="43">
+      <c r="A30" s="38">
         <v>7315</v>
       </c>
-      <c r="B30" s="43">
+      <c r="B30" s="38">
         <v>44660</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="38">
         <v>93786</v>
       </c>
-      <c r="D30" s="43">
+      <c r="D30" s="38">
         <v>80388</v>
       </c>
-      <c r="E30" s="43">
+      <c r="E30" s="38">
         <v>23751</v>
       </c>
       <c r="I30">
@@ -5436,36 +6857,36 @@
       <c r="J30">
         <v>19</v>
       </c>
-      <c r="L30" s="30">
+      <c r="L30" s="28">
         <v>9</v>
       </c>
-      <c r="M30" s="30">
+      <c r="M30" s="28">
         <v>40</v>
       </c>
-      <c r="N30" s="30">
+      <c r="N30" s="28">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="43">
+      <c r="A31" s="38">
         <v>5985</v>
       </c>
-      <c r="B31" s="43">
+      <c r="B31" s="38">
         <v>39900</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="38">
         <v>91350</v>
       </c>
-      <c r="D31" s="43">
+      <c r="D31" s="38">
         <v>85260</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="38">
         <v>27405</v>
       </c>
-      <c r="I31" s="30">
+      <c r="I31" s="28">
         <v>34</v>
       </c>
-      <c r="J31" s="30">
+      <c r="J31" s="28">
         <v>18</v>
       </c>
       <c r="L31">
@@ -5479,19 +6900,19 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="43">
+      <c r="A32" s="38">
         <v>4845</v>
       </c>
-      <c r="B32" s="43">
+      <c r="B32" s="38">
         <v>35340</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="38">
         <v>88350</v>
       </c>
-      <c r="D32" s="43">
+      <c r="D32" s="38">
         <v>89900</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="38">
         <v>31465</v>
       </c>
       <c r="I32">
@@ -5500,24 +6921,24 @@
       <c r="J32">
         <v>17</v>
       </c>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="43">
+      <c r="A33" s="38">
         <v>3876</v>
       </c>
-      <c r="B33" s="43">
+      <c r="B33" s="38">
         <v>31008</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="38">
         <v>84816</v>
       </c>
-      <c r="D33" s="43">
+      <c r="D33" s="38">
         <v>94240</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="38">
         <v>35960</v>
       </c>
       <c r="I33">
@@ -5528,45 +6949,45 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="43">
+      <c r="A34" s="38">
         <v>3060</v>
       </c>
-      <c r="B34" s="43">
+      <c r="B34" s="38">
         <v>26928</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="38">
         <v>80784</v>
       </c>
-      <c r="D34" s="43">
+      <c r="D34" s="38">
         <v>98208</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="38">
         <v>40920</v>
       </c>
-      <c r="I34" s="30">
+      <c r="I34" s="28">
         <v>37</v>
       </c>
-      <c r="J34" s="30">
+      <c r="J34" s="28">
         <v>15</v>
       </c>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="43">
+      <c r="A35" s="38">
         <v>2380</v>
       </c>
-      <c r="B35" s="43">
+      <c r="B35" s="38">
         <v>23120</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="38">
         <v>76296</v>
       </c>
-      <c r="D35" s="43">
+      <c r="D35" s="38">
         <v>101728</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="38">
         <v>46376</v>
       </c>
       <c r="I35">
@@ -5577,19 +6998,19 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="43">
+      <c r="A36" s="38">
         <v>1820</v>
       </c>
-      <c r="B36" s="45">
+      <c r="B36" s="40">
         <v>19600</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="38">
         <v>71400</v>
       </c>
-      <c r="D36" s="43">
+      <c r="D36" s="38">
         <v>104720</v>
       </c>
-      <c r="E36" s="43">
+      <c r="E36" s="38">
         <v>52360</v>
       </c>
       <c r="I36">
@@ -5598,47 +7019,47 @@
       <c r="J36">
         <v>13</v>
       </c>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="43">
+      <c r="A37" s="38">
         <v>1365</v>
       </c>
-      <c r="B37" s="43">
+      <c r="B37" s="38">
         <v>16380</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="38">
         <v>66150</v>
       </c>
-      <c r="D37" s="43">
+      <c r="D37" s="38">
         <v>107100</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="38">
         <v>58905</v>
       </c>
-      <c r="I37" s="30">
+      <c r="I37" s="28">
         <v>40</v>
       </c>
-      <c r="J37" s="30">
+      <c r="J37" s="28">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="43">
+      <c r="A38" s="38">
         <v>1001</v>
       </c>
-      <c r="B38" s="43">
+      <c r="B38" s="38">
         <v>13468</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="38">
         <v>60606</v>
       </c>
-      <c r="D38" s="43">
+      <c r="D38" s="38">
         <v>108780</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="38">
         <v>66045</v>
       </c>
       <c r="I38">
@@ -5647,24 +7068,24 @@
       <c r="J38">
         <v>11</v>
       </c>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="43">
+      <c r="A39" s="38">
         <v>715</v>
       </c>
-      <c r="B39" s="43">
+      <c r="B39" s="38">
         <v>10868</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="38">
         <v>54834</v>
       </c>
-      <c r="D39" s="44">
+      <c r="D39" s="39">
         <v>109668</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="38">
         <v>73815</v>
       </c>
       <c r="I39">
@@ -5675,45 +7096,45 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="43">
+      <c r="A40" s="38">
         <v>495</v>
       </c>
-      <c r="B40" s="43">
+      <c r="B40" s="38">
         <v>8580</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="38">
         <v>48906</v>
       </c>
-      <c r="D40" s="44">
+      <c r="D40" s="39">
         <v>109668</v>
       </c>
-      <c r="E40" s="43">
+      <c r="E40" s="38">
         <v>82251</v>
       </c>
-      <c r="I40" s="30">
+      <c r="I40" s="28">
         <v>43</v>
       </c>
-      <c r="J40" s="30">
+      <c r="J40" s="28">
         <v>9</v>
       </c>
-      <c r="L40" s="30"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="43">
+      <c r="A41" s="38">
         <v>330</v>
       </c>
-      <c r="B41" s="43">
+      <c r="B41" s="38">
         <v>6600</v>
       </c>
-      <c r="C41" s="43">
+      <c r="C41" s="38">
         <v>42900</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="38">
         <v>108680</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="38">
         <v>91390</v>
       </c>
       <c r="I41">
@@ -5724,19 +7145,19 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="43">
+      <c r="A42" s="38">
         <v>210</v>
       </c>
-      <c r="B42" s="43">
+      <c r="B42" s="38">
         <v>4920</v>
       </c>
-      <c r="C42" s="43">
+      <c r="C42" s="38">
         <v>36900</v>
       </c>
-      <c r="D42" s="43">
+      <c r="D42" s="38">
         <v>106600</v>
       </c>
-      <c r="E42" s="43">
+      <c r="E42" s="38">
         <v>101270</v>
       </c>
       <c r="I42">
@@ -5745,47 +7166,47 @@
       <c r="J42">
         <v>7</v>
       </c>
-      <c r="L42" s="30"/>
-      <c r="M42" s="30"/>
-      <c r="N42" s="30"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="43">
+      <c r="A43" s="38">
         <v>126</v>
       </c>
-      <c r="B43" s="43">
+      <c r="B43" s="38">
         <v>3528</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43" s="38">
         <v>30996</v>
       </c>
-      <c r="D43" s="43">
+      <c r="D43" s="38">
         <v>103320</v>
       </c>
-      <c r="E43" s="43">
+      <c r="E43" s="38">
         <v>111930</v>
       </c>
-      <c r="I43" s="30">
+      <c r="I43" s="28">
         <v>46</v>
       </c>
-      <c r="J43" s="30">
+      <c r="J43" s="28">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="43">
+      <c r="A44" s="38">
         <v>70</v>
       </c>
-      <c r="B44" s="43">
+      <c r="B44" s="38">
         <v>2408</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="38">
         <v>25284</v>
       </c>
-      <c r="D44" s="43">
+      <c r="D44" s="38">
         <v>98728</v>
       </c>
-      <c r="E44" s="43">
+      <c r="E44" s="38">
         <v>123410</v>
       </c>
       <c r="I44">
@@ -5794,24 +7215,24 @@
       <c r="J44">
         <v>5</v>
       </c>
-      <c r="L44" s="30"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="43">
+      <c r="A45" s="38">
         <v>35</v>
       </c>
-      <c r="B45" s="43">
+      <c r="B45" s="38">
         <v>1540</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="38">
         <v>19866</v>
       </c>
-      <c r="D45" s="43">
+      <c r="D45" s="38">
         <v>92708</v>
       </c>
-      <c r="E45" s="43">
+      <c r="E45" s="38">
         <v>135751</v>
       </c>
       <c r="I45">
@@ -5822,45 +7243,45 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="43">
+      <c r="A46" s="38">
         <v>15</v>
       </c>
-      <c r="B46" s="43">
+      <c r="B46" s="38">
         <v>900</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="38">
         <v>14850</v>
       </c>
-      <c r="D46" s="43">
+      <c r="D46" s="38">
         <v>85140</v>
       </c>
-      <c r="E46" s="43">
+      <c r="E46" s="38">
         <v>148995</v>
       </c>
-      <c r="I46" s="30">
+      <c r="I46" s="28">
         <v>49</v>
       </c>
-      <c r="J46" s="30">
+      <c r="J46" s="28">
         <v>3</v>
       </c>
-      <c r="L46" s="30"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="43">
+      <c r="A47" s="38">
         <v>5</v>
       </c>
-      <c r="B47" s="43">
+      <c r="B47" s="38">
         <v>460</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="38">
         <v>10350</v>
       </c>
-      <c r="D47" s="43">
+      <c r="D47" s="38">
         <v>75900</v>
       </c>
-      <c r="E47" s="43">
+      <c r="E47" s="38">
         <v>163185</v>
       </c>
       <c r="I47">
@@ -5871,104 +7292,104 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="43">
+      <c r="A48" s="38">
         <v>1</v>
       </c>
-      <c r="B48" s="43">
+      <c r="B48" s="38">
         <v>188</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="38">
         <v>6486</v>
       </c>
-      <c r="D48" s="43">
+      <c r="D48" s="38">
         <v>64860</v>
       </c>
-      <c r="E48" s="43">
+      <c r="E48" s="38">
         <v>178365</v>
       </c>
       <c r="I48">
         <v>51</v>
       </c>
-      <c r="J48" s="56">
+      <c r="J48" s="50">
         <v>1</v>
       </c>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49" s="43">
+      <c r="A49" s="38">
         <v>0</v>
       </c>
-      <c r="B49" s="43">
+      <c r="B49" s="38">
         <v>48</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="38">
         <v>3384</v>
       </c>
-      <c r="D49" s="43">
+      <c r="D49" s="38">
         <v>51888</v>
       </c>
-      <c r="E49" s="43">
+      <c r="E49" s="38">
         <v>194580</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="43">
+      <c r="A50" s="38">
         <v>0</v>
       </c>
-      <c r="B50" s="43">
+      <c r="B50" s="38">
         <v>0</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="38">
         <v>1176</v>
       </c>
-      <c r="D50" s="43">
+      <c r="D50" s="38">
         <v>36848</v>
       </c>
-      <c r="E50" s="43">
+      <c r="E50" s="38">
         <v>211876</v>
       </c>
-      <c r="L50" s="30"/>
-      <c r="M50" s="30"/>
-      <c r="N50" s="30"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="28"/>
+      <c r="N50" s="28"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51" s="43">
+      <c r="A51" s="38">
         <v>0</v>
       </c>
-      <c r="B51" s="43">
+      <c r="B51" s="38">
         <v>0</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="38">
         <v>0</v>
       </c>
-      <c r="D51" s="45">
+      <c r="D51" s="40">
         <v>19600</v>
       </c>
-      <c r="E51" s="43">
+      <c r="E51" s="38">
         <v>230300</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52" s="43">
+      <c r="A52" s="38">
         <v>0</v>
       </c>
-      <c r="B52" s="43">
+      <c r="B52" s="38">
         <v>0</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52" s="38">
         <v>0</v>
       </c>
-      <c r="D52" s="43">
+      <c r="D52" s="38">
         <v>0</v>
       </c>
-      <c r="E52" s="43">
+      <c r="E52" s="38">
         <v>249900</v>
       </c>
-      <c r="L52" s="30"/>
-      <c r="M52" s="30"/>
-      <c r="N52" s="30"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>